<commit_message>
ajout d'une deuxième version de plannification avec répartition des tâches
</commit_message>
<xml_diff>
--- a/PlannificationDevMobile.xlsx
+++ b/PlannificationDevMobile.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael.schaffo\HE-ARC\MODULE NIVEAU III\Devellopement Mobile\Projets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lancelot\Documents\Depots\StayFitAndroid\StayFit-Android-Part\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Phase d'introduction </t>
   </si>
@@ -78,6 +78,27 @@
   </si>
   <si>
     <t>Optimiser les ressources</t>
+  </si>
+  <si>
+    <t>Distribution des tâches</t>
+  </si>
+  <si>
+    <t>Schaffo</t>
+  </si>
+  <si>
+    <t>Gygi</t>
+  </si>
+  <si>
+    <t>Magnin</t>
+  </si>
+  <si>
+    <t>Tous</t>
+  </si>
+  <si>
+    <t>fonctionnalités suplémentaires</t>
+  </si>
+  <si>
+    <t>integré une map avec position GPS</t>
   </si>
 </sst>
 </file>
@@ -101,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,24 +143,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF33CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,11 +195,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,15 +220,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF33CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -495,16 +561,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q20"/>
+  <dimension ref="A2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.28515625" customWidth="1"/>
-    <col min="2" max="17" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="57.25" customWidth="1"/>
+    <col min="2" max="17" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -582,7 +648,7 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -603,7 +669,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -646,8 +712,8 @@
         <v>5</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -668,8 +734,8 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -711,10 +777,10 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -733,8 +799,8 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -756,9 +822,9 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -778,10 +844,10 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -802,8 +868,8 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -846,7 +912,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="6"/>
+      <c r="N16" s="12"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -867,7 +933,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="6"/>
+      <c r="N17" s="12"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -888,7 +954,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="6"/>
+      <c r="N18" s="12"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -931,11 +997,97 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
       <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>